<commit_message>
add inital Chrome script that contains a function to get an extension, add inital Excel script to convert to and from CSV, update Excel template for hardware survey
</commit_message>
<xml_diff>
--- a/Hardware/Template.xlsx
+++ b/Hardware/Template.xlsx
@@ -4,22 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Model</t>
   </si>
@@ -112,106 +107,13 @@
   </si>
   <si>
     <t>WHCP version (Q30)</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
-    <t>A8</t>
-  </si>
-  <si>
-    <t>A9</t>
-  </si>
-  <si>
-    <t>A10</t>
-  </si>
-  <si>
-    <t>A11</t>
-  </si>
-  <si>
-    <t>A12</t>
-  </si>
-  <si>
-    <t>A13</t>
-  </si>
-  <si>
-    <t>A14</t>
-  </si>
-  <si>
-    <t>A15</t>
-  </si>
-  <si>
-    <t>A16</t>
-  </si>
-  <si>
-    <t>A17</t>
-  </si>
-  <si>
-    <t>A18</t>
-  </si>
-  <si>
-    <t>A19</t>
-  </si>
-  <si>
-    <t>A20</t>
-  </si>
-  <si>
-    <t>A21</t>
-  </si>
-  <si>
-    <t>A22</t>
-  </si>
-  <si>
-    <t>A23</t>
-  </si>
-  <si>
-    <t>A24</t>
-  </si>
-  <si>
-    <t>A25</t>
-  </si>
-  <si>
-    <t>A26</t>
-  </si>
-  <si>
-    <t>A27</t>
-  </si>
-  <si>
-    <t>A28</t>
-  </si>
-  <si>
-    <t>A29</t>
-  </si>
-  <si>
-    <t>A30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,16 +121,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -236,15 +438,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -522,47 +913,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE6" sqref="AE6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -659,103 +1016,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" t="s">
-        <v>49</v>
-      </c>
-      <c r="T2" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" t="s">
-        <v>52</v>
-      </c>
-      <c r="W2" t="s">
-        <v>53</v>
-      </c>
-      <c r="X2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>61</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>